<commit_message>
Further transaction volume updates
</commit_message>
<xml_diff>
--- a/data/processed/202308-services-list-processed - jbedits.xlsx
+++ b/data/processed/202308-services-list-processed - jbedits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Turing\Projects\decision-services-index\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ACB036-A3FC-49AF-9564-FBE61A244DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8B823C-BA6D-468C-B1D9-568AA330A97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3375" uniqueCount="1087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3542" uniqueCount="1111">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -3296,7 +3296,79 @@
     <t>Appears that this is a newly separate benefit</t>
   </si>
   <si>
+    <t>UP TO HERE</t>
+  </si>
+  <si>
     <t>Have taken the number for enhanced criminal record check from archive, which is actually the link for the DBS</t>
+  </si>
+  <si>
+    <t>Apprenticeships: vacancies posted</t>
+  </si>
+  <si>
+    <t>Skills Funding Agency (SFA) learning and training: training organisation data returns</t>
+  </si>
+  <si>
+    <t>present on web archive but no data</t>
+  </si>
+  <si>
+    <t>Rod catch returns: salmon and sea trout catches</t>
+  </si>
+  <si>
+    <t>Not clear what services this groups together</t>
+  </si>
+  <si>
+    <t>Registrations to receive flood warnings</t>
+  </si>
+  <si>
+    <t>Flood warnings is included below</t>
+  </si>
+  <si>
+    <t>There is a record for fluorinated gas but it is included below</t>
+  </si>
+  <si>
+    <t>Registrations of waste carriers, brokers and dealers</t>
+  </si>
+  <si>
+    <t>There are a couple of other waste related things on the archive, but neither relate to exemptions specifically</t>
+  </si>
+  <si>
+    <t>Certificates of no impediment to marriage abroad</t>
+  </si>
+  <si>
+    <t>There is a pay service on the website but no data</t>
+  </si>
+  <si>
+    <t>Legalisation and Apostille certificate applications</t>
+  </si>
+  <si>
+    <t>there is a record for misc consular services</t>
+  </si>
+  <si>
+    <t>Orders for a copy of a birth, death or marriage certificate</t>
+  </si>
+  <si>
+    <t>present on the website but no data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">present on the website but no data. Not clear for internet how many individual payments there are, you can pay annually or per trip, etc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">present on website but no data. This doesn't cover all benefits but is a reasonable approximation. </t>
+  </si>
+  <si>
+    <t>Data on divorce applications but not responses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">present on the website but no data.  </t>
+  </si>
+  <si>
+    <t>present on the website but no data. This is data for all sent out, not replies, but seems a reasonable approximation</t>
+  </si>
+  <si>
+    <t>HMRC put no data on the website and only three transactions in the spreadsheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No obviously available online statistics on how many returnes are filed, just on receipts </t>
   </si>
 </sst>
 </file>
@@ -3683,10 +3755,10 @@
   <dimension ref="A1:W378"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C147" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B257" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H162" sqref="H162"/>
+      <selection pane="bottomRight" activeCell="H266" sqref="H266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3695,7 +3767,8 @@
     <col min="3" max="3" width="40.1796875" customWidth="1"/>
     <col min="4" max="4" width="12.1796875" customWidth="1"/>
     <col min="5" max="5" width="16.40625" customWidth="1"/>
-    <col min="6" max="7" width="20.76953125" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" customWidth="1"/>
     <col min="8" max="8" width="40.953125" customWidth="1"/>
     <col min="9" max="9" width="20.04296875" customWidth="1"/>
   </cols>
@@ -11136,7 +11209,7 @@
         <v>3921728</v>
       </c>
       <c r="H148" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="I148">
         <v>1012591</v>
@@ -12947,6 +13020,12 @@
       <c r="C185" t="s">
         <v>520</v>
       </c>
+      <c r="E185" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F185" t="s">
+        <v>1037</v>
+      </c>
       <c r="I185">
         <v>5988</v>
       </c>
@@ -12988,6 +13067,15 @@
       <c r="C186" t="s">
         <v>535</v>
       </c>
+      <c r="E186" t="s">
+        <v>1088</v>
+      </c>
+      <c r="F186" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H186" t="s">
+        <v>1053</v>
+      </c>
       <c r="I186">
         <v>66885</v>
       </c>
@@ -13029,6 +13117,12 @@
       <c r="C187" t="s">
         <v>544</v>
       </c>
+      <c r="E187" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F187" t="s">
+        <v>1037</v>
+      </c>
       <c r="I187">
         <v>10879</v>
       </c>
@@ -13070,6 +13164,15 @@
       <c r="C188" t="s">
         <v>554</v>
       </c>
+      <c r="E188" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F188" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H188" t="s">
+        <v>1053</v>
+      </c>
       <c r="I188">
         <v>620</v>
       </c>
@@ -13111,6 +13214,12 @@
       <c r="C189" t="s">
         <v>981</v>
       </c>
+      <c r="E189" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F189" t="s">
+        <v>1037</v>
+      </c>
       <c r="I189">
         <v>33894</v>
       </c>
@@ -13152,6 +13261,12 @@
       <c r="C190" t="s">
         <v>985</v>
       </c>
+      <c r="E190" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F190" t="s">
+        <v>1037</v>
+      </c>
       <c r="I190">
         <v>70188</v>
       </c>
@@ -13193,6 +13308,15 @@
       <c r="C191" t="s">
         <v>183</v>
       </c>
+      <c r="E191" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F191" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H191" t="s">
+        <v>1090</v>
+      </c>
       <c r="I191">
         <v>3270</v>
       </c>
@@ -13246,6 +13370,12 @@
       <c r="C192" t="s">
         <v>220</v>
       </c>
+      <c r="F192">
+        <v>15118</v>
+      </c>
+      <c r="H192" t="s">
+        <v>1091</v>
+      </c>
       <c r="I192">
         <v>10985</v>
       </c>
@@ -13287,6 +13417,15 @@
       <c r="C193" t="s">
         <v>566</v>
       </c>
+      <c r="E193" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F193" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H193" t="s">
+        <v>1092</v>
+      </c>
       <c r="I193">
         <v>1946</v>
       </c>
@@ -13332,7 +13471,10 @@
         <v>570</v>
       </c>
       <c r="E194" t="s">
-        <v>570</v>
+        <v>1037</v>
+      </c>
+      <c r="F194" t="s">
+        <v>1037</v>
       </c>
       <c r="I194">
         <v>230</v>
@@ -13375,6 +13517,15 @@
       <c r="C195" t="s">
         <v>572</v>
       </c>
+      <c r="E195" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F195" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H195" t="s">
+        <v>1095</v>
+      </c>
       <c r="I195">
         <v>231</v>
       </c>
@@ -13416,6 +13567,12 @@
       <c r="C196" t="s">
         <v>574</v>
       </c>
+      <c r="E196" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F196" t="s">
+        <v>1037</v>
+      </c>
       <c r="I196">
         <v>231</v>
       </c>
@@ -13457,6 +13614,15 @@
       <c r="C197" t="s">
         <v>576</v>
       </c>
+      <c r="E197" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F197" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H197" t="s">
+        <v>1094</v>
+      </c>
       <c r="I197">
         <v>193213</v>
       </c>
@@ -13498,6 +13664,12 @@
       <c r="C198" t="s">
         <v>581</v>
       </c>
+      <c r="E198" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F198" t="s">
+        <v>1037</v>
+      </c>
       <c r="I198">
         <v>34990</v>
       </c>
@@ -13539,6 +13711,12 @@
       <c r="C199" t="s">
         <v>599</v>
       </c>
+      <c r="E199" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F199" t="s">
+        <v>1037</v>
+      </c>
       <c r="I199">
         <v>14135</v>
       </c>
@@ -13580,6 +13758,12 @@
       <c r="C200" t="s">
         <v>606</v>
       </c>
+      <c r="E200" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F200" t="s">
+        <v>1037</v>
+      </c>
       <c r="I200">
         <v>1583</v>
       </c>
@@ -13621,6 +13805,12 @@
       <c r="C201" t="s">
         <v>608</v>
       </c>
+      <c r="E201" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F201" t="s">
+        <v>1037</v>
+      </c>
       <c r="I201">
         <v>684</v>
       </c>
@@ -13662,6 +13852,15 @@
       <c r="C202" t="s">
         <v>610</v>
       </c>
+      <c r="E202" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F202" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H202" t="s">
+        <v>1097</v>
+      </c>
       <c r="I202">
         <v>14577</v>
       </c>
@@ -13703,6 +13902,12 @@
       <c r="C203" t="s">
         <v>612</v>
       </c>
+      <c r="E203" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F203" t="s">
+        <v>1037</v>
+      </c>
       <c r="J203" t="s">
         <v>613</v>
       </c>
@@ -13741,6 +13946,9 @@
       <c r="C204" t="s">
         <v>616</v>
       </c>
+      <c r="E204" t="s">
+        <v>570</v>
+      </c>
       <c r="I204">
         <v>414</v>
       </c>
@@ -13782,6 +13990,15 @@
       <c r="C205" t="s">
         <v>618</v>
       </c>
+      <c r="E205" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F205" s="2">
+        <v>32787</v>
+      </c>
+      <c r="H205" t="s">
+        <v>1093</v>
+      </c>
       <c r="I205">
         <v>39061</v>
       </c>
@@ -13823,6 +14040,12 @@
       <c r="C206" t="s">
         <v>990</v>
       </c>
+      <c r="E206" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F206" t="s">
+        <v>1037</v>
+      </c>
       <c r="I206">
         <v>616708</v>
       </c>
@@ -13914,6 +14137,15 @@
       <c r="C208" t="s">
         <v>997</v>
       </c>
+      <c r="E208" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F208">
+        <v>58220</v>
+      </c>
+      <c r="H208" t="s">
+        <v>1096</v>
+      </c>
       <c r="I208">
         <v>57316</v>
       </c>
@@ -13959,7 +14191,13 @@
         <v>67</v>
       </c>
       <c r="E209" t="s">
-        <v>67</v>
+        <v>1098</v>
+      </c>
+      <c r="F209" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H209" t="s">
+        <v>1099</v>
       </c>
       <c r="J209" t="s">
         <v>68</v>
@@ -14005,6 +14243,12 @@
       <c r="E210" t="s">
         <v>72</v>
       </c>
+      <c r="F210" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H210" t="s">
+        <v>1099</v>
+      </c>
       <c r="I210">
         <v>1665</v>
       </c>
@@ -14052,6 +14296,12 @@
       <c r="E211" t="s">
         <v>75</v>
       </c>
+      <c r="F211" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H211" t="s">
+        <v>1099</v>
+      </c>
       <c r="J211" t="s">
         <v>76</v>
       </c>
@@ -14096,6 +14346,12 @@
       <c r="E212" t="s">
         <v>488</v>
       </c>
+      <c r="F212" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H212" t="s">
+        <v>1047</v>
+      </c>
       <c r="I212">
         <v>39764</v>
       </c>
@@ -14143,6 +14399,12 @@
       <c r="E213" t="s">
         <v>746</v>
       </c>
+      <c r="F213" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H213" t="s">
+        <v>1047</v>
+      </c>
       <c r="I213">
         <v>124017</v>
       </c>
@@ -14190,6 +14452,12 @@
       <c r="E214" t="s">
         <v>750</v>
       </c>
+      <c r="F214" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H214" t="s">
+        <v>1047</v>
+      </c>
       <c r="I214">
         <v>10662</v>
       </c>
@@ -14234,6 +14502,9 @@
       <c r="C215" t="s">
         <v>762</v>
       </c>
+      <c r="F215" t="s">
+        <v>1037</v>
+      </c>
       <c r="J215" t="s">
         <v>763</v>
       </c>
@@ -14275,6 +14546,15 @@
       <c r="C216" t="s">
         <v>769</v>
       </c>
+      <c r="E216" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F216" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H216" t="s">
+        <v>1047</v>
+      </c>
       <c r="I216">
         <v>253487</v>
       </c>
@@ -14316,6 +14596,12 @@
       <c r="C217" t="s">
         <v>771</v>
       </c>
+      <c r="E217" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F217" t="s">
+        <v>1037</v>
+      </c>
       <c r="I217">
         <v>831</v>
       </c>
@@ -14360,6 +14646,15 @@
       <c r="C218" t="s">
         <v>776</v>
       </c>
+      <c r="E218" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F218" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H218" t="s">
+        <v>1101</v>
+      </c>
       <c r="I218">
         <v>10221</v>
       </c>
@@ -14404,6 +14699,12 @@
       <c r="C219" t="s">
         <v>852</v>
       </c>
+      <c r="E219" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F219" t="s">
+        <v>1037</v>
+      </c>
       <c r="J219" t="s">
         <v>853</v>
       </c>
@@ -14445,6 +14746,12 @@
       <c r="C220" t="s">
         <v>1002</v>
       </c>
+      <c r="E220" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F220" t="s">
+        <v>1037</v>
+      </c>
       <c r="I220">
         <v>13193</v>
       </c>
@@ -14490,7 +14797,13 @@
         <v>928</v>
       </c>
       <c r="E221" t="s">
-        <v>928</v>
+        <v>1037</v>
+      </c>
+      <c r="F221" s="2">
+        <v>1327057</v>
+      </c>
+      <c r="H221" t="s">
+        <v>1102</v>
       </c>
       <c r="I221">
         <v>1608817</v>
@@ -14533,6 +14846,12 @@
       <c r="C222" t="s">
         <v>876</v>
       </c>
+      <c r="E222" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F222" t="s">
+        <v>1037</v>
+      </c>
       <c r="I222">
         <v>388</v>
       </c>
@@ -14574,6 +14893,12 @@
       <c r="C223" t="s">
         <v>882</v>
       </c>
+      <c r="E223" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F223" t="s">
+        <v>1037</v>
+      </c>
       <c r="I223">
         <v>137</v>
       </c>
@@ -14615,6 +14940,12 @@
       <c r="C224" t="s">
         <v>890</v>
       </c>
+      <c r="E224" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F224" t="s">
+        <v>1037</v>
+      </c>
       <c r="I224">
         <v>1439</v>
       </c>
@@ -14656,6 +14987,12 @@
       <c r="C225" t="s">
         <v>842</v>
       </c>
+      <c r="E225" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F225" t="s">
+        <v>1037</v>
+      </c>
       <c r="I225">
         <v>7127</v>
       </c>
@@ -14706,6 +15043,12 @@
       <c r="E226" t="s">
         <v>443</v>
       </c>
+      <c r="F226" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H226" t="s">
+        <v>1104</v>
+      </c>
       <c r="I226">
         <v>6852544</v>
       </c>
@@ -14746,6 +15089,15 @@
       </c>
       <c r="C227" t="s">
         <v>20</v>
+      </c>
+      <c r="E227" t="s">
+        <v>313</v>
+      </c>
+      <c r="F227" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H227" t="s">
+        <v>1105</v>
       </c>
       <c r="I227">
         <v>166877</v>
@@ -14788,6 +15140,15 @@
       <c r="C228" t="s">
         <v>77</v>
       </c>
+      <c r="E228" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F228" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H228" t="s">
+        <v>1106</v>
+      </c>
       <c r="I228">
         <v>129028</v>
       </c>
@@ -14835,6 +15196,12 @@
       <c r="E229" t="s">
         <v>317</v>
       </c>
+      <c r="F229" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H229" t="s">
+        <v>1107</v>
+      </c>
       <c r="I229">
         <v>317453</v>
       </c>
@@ -14882,6 +15249,12 @@
       <c r="E230" t="s">
         <v>353</v>
       </c>
+      <c r="F230" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H230" t="s">
+        <v>1103</v>
+      </c>
       <c r="I230">
         <v>87117</v>
       </c>
@@ -14929,6 +15302,12 @@
       <c r="E231" t="s">
         <v>358</v>
       </c>
+      <c r="F231" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H231" t="s">
+        <v>1103</v>
+      </c>
       <c r="I231">
         <v>433472</v>
       </c>
@@ -14976,6 +15355,12 @@
       <c r="E232" t="s">
         <v>361</v>
       </c>
+      <c r="F232" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H232" t="s">
+        <v>1108</v>
+      </c>
       <c r="I232">
         <v>184716</v>
       </c>
@@ -15023,6 +15408,12 @@
       <c r="E233" t="s">
         <v>786</v>
       </c>
+      <c r="F233" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H233" t="s">
+        <v>1103</v>
+      </c>
       <c r="I233">
         <v>18563</v>
       </c>
@@ -15064,6 +15455,12 @@
       <c r="C234" t="s">
         <v>760</v>
       </c>
+      <c r="E234" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F234" t="s">
+        <v>1037</v>
+      </c>
       <c r="I234">
         <v>109350</v>
       </c>
@@ -15105,6 +15502,15 @@
       <c r="C235" t="s">
         <v>33</v>
       </c>
+      <c r="E235" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F235" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H235" t="s">
+        <v>1109</v>
+      </c>
       <c r="I235">
         <v>440167</v>
       </c>
@@ -15146,6 +15552,12 @@
       <c r="C236" t="s">
         <v>116</v>
       </c>
+      <c r="E236" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F236" t="s">
+        <v>1037</v>
+      </c>
       <c r="I236">
         <v>1019495</v>
       </c>
@@ -15190,6 +15602,12 @@
       <c r="C237" t="s">
         <v>121</v>
       </c>
+      <c r="E237" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F237" t="s">
+        <v>1037</v>
+      </c>
       <c r="I237">
         <v>326786</v>
       </c>
@@ -15234,6 +15652,12 @@
       <c r="C238" t="s">
         <v>127</v>
       </c>
+      <c r="E238" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F238" t="s">
+        <v>1037</v>
+      </c>
       <c r="I238">
         <v>17311</v>
       </c>
@@ -15278,6 +15702,12 @@
       <c r="C239" t="s">
         <v>130</v>
       </c>
+      <c r="E239" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F239" t="s">
+        <v>1037</v>
+      </c>
       <c r="I239">
         <v>9820</v>
       </c>
@@ -15322,6 +15752,15 @@
       <c r="C240" t="s">
         <v>155</v>
       </c>
+      <c r="E240" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F240" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H240" t="s">
+        <v>1110</v>
+      </c>
       <c r="I240">
         <v>360298</v>
       </c>
@@ -15375,6 +15814,12 @@
       <c r="C241" t="s">
         <v>166</v>
       </c>
+      <c r="E241" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F241" t="s">
+        <v>1037</v>
+      </c>
       <c r="I241">
         <v>1019041</v>
       </c>
@@ -15428,6 +15873,12 @@
       <c r="C242" t="s">
         <v>172</v>
       </c>
+      <c r="E242" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F242" t="s">
+        <v>1037</v>
+      </c>
       <c r="I242">
         <v>148961</v>
       </c>
@@ -15481,6 +15932,12 @@
       <c r="C243" t="s">
         <v>195</v>
       </c>
+      <c r="E243" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F243" t="s">
+        <v>1037</v>
+      </c>
       <c r="I243">
         <v>6716</v>
       </c>
@@ -15534,6 +15991,12 @@
       <c r="C244" t="s">
         <v>229</v>
       </c>
+      <c r="E244" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F244" t="s">
+        <v>1037</v>
+      </c>
       <c r="I244">
         <v>351337</v>
       </c>
@@ -15575,6 +16038,12 @@
       <c r="C245" t="s">
         <v>411</v>
       </c>
+      <c r="E245" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F245" t="s">
+        <v>1037</v>
+      </c>
       <c r="I245">
         <v>108633</v>
       </c>
@@ -15616,6 +16085,12 @@
       <c r="C246" t="s">
         <v>641</v>
       </c>
+      <c r="E246" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F246" t="s">
+        <v>1037</v>
+      </c>
       <c r="I246">
         <v>22986</v>
       </c>
@@ -15660,6 +16135,12 @@
       <c r="C247" t="s">
         <v>682</v>
       </c>
+      <c r="E247" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F247" t="s">
+        <v>1037</v>
+      </c>
       <c r="I247">
         <v>224072</v>
       </c>
@@ -15713,6 +16194,12 @@
       <c r="C248" t="s">
         <v>687</v>
       </c>
+      <c r="E248" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F248" t="s">
+        <v>1037</v>
+      </c>
       <c r="I248">
         <v>1764</v>
       </c>
@@ -15757,6 +16244,12 @@
       <c r="C249" t="s">
         <v>690</v>
       </c>
+      <c r="E249" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F249" t="s">
+        <v>1037</v>
+      </c>
       <c r="I249">
         <v>5108079</v>
       </c>
@@ -15798,6 +16291,12 @@
       <c r="C250" t="s">
         <v>692</v>
       </c>
+      <c r="E250" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F250" t="s">
+        <v>1037</v>
+      </c>
       <c r="J250" t="s">
         <v>693</v>
       </c>
@@ -15839,6 +16338,12 @@
       <c r="C251" t="s">
         <v>698</v>
       </c>
+      <c r="E251" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F251" t="s">
+        <v>1037</v>
+      </c>
       <c r="I251">
         <v>584286</v>
       </c>
@@ -15892,6 +16397,12 @@
       <c r="C252" t="s">
         <v>712</v>
       </c>
+      <c r="E252" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F252" t="s">
+        <v>1037</v>
+      </c>
       <c r="I252">
         <v>1054826</v>
       </c>
@@ -15945,6 +16456,12 @@
       <c r="C253" t="s">
         <v>714</v>
       </c>
+      <c r="E253" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F253" t="s">
+        <v>1037</v>
+      </c>
       <c r="I253">
         <v>5733</v>
       </c>
@@ -15989,6 +16506,12 @@
       <c r="C254" t="s">
         <v>717</v>
       </c>
+      <c r="E254" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F254" t="s">
+        <v>1037</v>
+      </c>
       <c r="I254">
         <v>1710581</v>
       </c>
@@ -16033,6 +16556,12 @@
       <c r="C255" t="s">
         <v>725</v>
       </c>
+      <c r="E255" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F255" t="s">
+        <v>1037</v>
+      </c>
       <c r="I255">
         <v>15088</v>
       </c>
@@ -16086,6 +16615,12 @@
       <c r="C256" t="s">
         <v>727</v>
       </c>
+      <c r="E256" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F256" t="s">
+        <v>1037</v>
+      </c>
       <c r="I256">
         <v>10153</v>
       </c>
@@ -16130,6 +16665,12 @@
       <c r="C257" t="s">
         <v>730</v>
       </c>
+      <c r="E257" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F257" t="s">
+        <v>1037</v>
+      </c>
       <c r="J257" t="s">
         <v>731</v>
       </c>
@@ -16168,6 +16709,12 @@
       <c r="C258" t="s">
         <v>732</v>
       </c>
+      <c r="E258" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F258" t="s">
+        <v>1037</v>
+      </c>
       <c r="I258">
         <v>466</v>
       </c>
@@ -16221,6 +16768,12 @@
       <c r="C259" t="s">
         <v>734</v>
       </c>
+      <c r="E259" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F259" t="s">
+        <v>1037</v>
+      </c>
       <c r="I259">
         <v>57128</v>
       </c>
@@ -16274,6 +16827,12 @@
       <c r="C260" t="s">
         <v>736</v>
       </c>
+      <c r="E260" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F260" t="s">
+        <v>1037</v>
+      </c>
       <c r="I260">
         <v>20917</v>
       </c>
@@ -16327,6 +16886,12 @@
       <c r="C261" t="s">
         <v>741</v>
       </c>
+      <c r="E261" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F261" t="s">
+        <v>1037</v>
+      </c>
       <c r="I261">
         <v>7365</v>
       </c>
@@ -16368,6 +16933,12 @@
       <c r="C262" t="s">
         <v>1020</v>
       </c>
+      <c r="E262" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F262" t="s">
+        <v>1037</v>
+      </c>
       <c r="I262">
         <v>9591</v>
       </c>
@@ -16409,6 +16980,12 @@
       <c r="C263" t="s">
         <v>1022</v>
       </c>
+      <c r="E263" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F263" t="s">
+        <v>1037</v>
+      </c>
       <c r="I263">
         <v>1103739</v>
       </c>
@@ -16450,6 +17027,12 @@
       <c r="C264" t="s">
         <v>1024</v>
       </c>
+      <c r="E264" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F264" t="s">
+        <v>1037</v>
+      </c>
       <c r="I264">
         <v>2700716</v>
       </c>
@@ -16496,6 +17079,9 @@
       </c>
       <c r="E265" t="s">
         <v>289</v>
+      </c>
+      <c r="H265" t="s">
+        <v>1086</v>
       </c>
       <c r="I265">
         <v>18299</v>

</xml_diff>

<commit_message>
Update 202308-services-list-processed - jbedits.xlsx
</commit_message>
<xml_diff>
--- a/data/processed/202308-services-list-processed - jbedits.xlsx
+++ b/data/processed/202308-services-list-processed - jbedits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Turing\Projects\decision-services-index\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8B823C-BA6D-468C-B1D9-568AA330A97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDFCECB-6985-40FD-AD24-5000DE42995D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3542" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="1139">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -3296,9 +3296,6 @@
     <t>Appears that this is a newly separate benefit</t>
   </si>
   <si>
-    <t>UP TO HERE</t>
-  </si>
-  <si>
     <t>Have taken the number for enhanced criminal record check from archive, which is actually the link for the DBS</t>
   </si>
   <si>
@@ -3369,6 +3366,93 @@
   </si>
   <si>
     <t xml:space="preserve">No obviously available online statistics on how many returnes are filed, just on receipts </t>
+  </si>
+  <si>
+    <t>this exists</t>
+  </si>
+  <si>
+    <t>Council tax valuations appeal. Now with the valuations office agency</t>
+  </si>
+  <si>
+    <t>On the website but no data. Now at the valuation office agency. There is an entry for fair rent cases but this is something different</t>
+  </si>
+  <si>
+    <t>Reports of immigration and commodity abuse</t>
+  </si>
+  <si>
+    <t>Applies to visa applications. Not found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On the website but no data </t>
+  </si>
+  <si>
+    <t>On website but no data</t>
+  </si>
+  <si>
+    <t>Registered traveller service</t>
+  </si>
+  <si>
+    <t>On the website but no data</t>
+  </si>
+  <si>
+    <t>Have added domestic and international passport application figures</t>
+  </si>
+  <si>
+    <t>Innovate UK funding: applications for grants</t>
+  </si>
+  <si>
+    <t>Applications for bankruptcy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debt Relief Order (DRO) applications. Name has changed. </t>
+  </si>
+  <si>
+    <t>Thoroughly checked similar ones but income payment agreements are for paying back your debts when employed</t>
+  </si>
+  <si>
+    <t>Redundancy Payments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conduct of directors assessments </t>
+  </si>
+  <si>
+    <t>Patent renewals (F12) + Trade mark renewals + Designs: registered design renewals</t>
+  </si>
+  <si>
+    <t>Present on website but no data. Note that a design is not a patent</t>
+  </si>
+  <si>
+    <t>Lots of trade mark data but nothing about tracking</t>
+  </si>
+  <si>
+    <t>Applications for orphan work but not viewing register</t>
+  </si>
+  <si>
+    <t>Land Registry: title register, plan and document views (if you click through it is the same service)</t>
+  </si>
+  <si>
+    <t>Seems to be a new service</t>
+  </si>
+  <si>
+    <t>dataset access service</t>
+  </si>
+  <si>
+    <t>Should add together the three cells for applying for legal aid from the historical dataset</t>
+  </si>
+  <si>
+    <t>Legal aid in civil cases: acts of assistance, + 2 other similar rows to update</t>
+  </si>
+  <si>
+    <t>Not the same as salmon rod catches which are used above</t>
+  </si>
+  <si>
+    <t>No data on website</t>
+  </si>
+  <si>
+    <t>Minor tribunal claims</t>
+  </si>
+  <si>
+    <t>This tribunal was rolled up into minor tribunal claims with a lot of other tribunal types. Make sure to only use this once here. No data on website</t>
   </si>
 </sst>
 </file>
@@ -3755,10 +3839,10 @@
   <dimension ref="A1:W378"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B257" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B312" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H266" sqref="H266"/>
+      <selection pane="bottomRight" activeCell="A320" sqref="A320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -11209,7 +11293,7 @@
         <v>3921728</v>
       </c>
       <c r="H148" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="I148">
         <v>1012591</v>
@@ -13068,7 +13152,7 @@
         <v>535</v>
       </c>
       <c r="E186" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="F186" t="s">
         <v>1037</v>
@@ -13165,7 +13249,7 @@
         <v>554</v>
       </c>
       <c r="E188" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="F188" t="s">
         <v>1037</v>
@@ -13315,7 +13399,7 @@
         <v>1037</v>
       </c>
       <c r="H191" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="I191">
         <v>3270</v>
@@ -13374,7 +13458,7 @@
         <v>15118</v>
       </c>
       <c r="H192" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="I192">
         <v>10985</v>
@@ -13424,7 +13508,7 @@
         <v>1037</v>
       </c>
       <c r="H193" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="I193">
         <v>1946</v>
@@ -13524,7 +13608,7 @@
         <v>1037</v>
       </c>
       <c r="H195" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="I195">
         <v>231</v>
@@ -13621,7 +13705,7 @@
         <v>1037</v>
       </c>
       <c r="H197" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="I197">
         <v>193213</v>
@@ -13859,7 +13943,7 @@
         <v>1037</v>
       </c>
       <c r="H202" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="I202">
         <v>14577</v>
@@ -13997,7 +14081,7 @@
         <v>32787</v>
       </c>
       <c r="H205" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="I205">
         <v>39061</v>
@@ -14144,7 +14228,7 @@
         <v>58220</v>
       </c>
       <c r="H208" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="I208">
         <v>57316</v>
@@ -14191,13 +14275,13 @@
         <v>67</v>
       </c>
       <c r="E209" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F209" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H209" t="s">
         <v>1098</v>
-      </c>
-      <c r="F209" t="s">
-        <v>1037</v>
-      </c>
-      <c r="H209" t="s">
-        <v>1099</v>
       </c>
       <c r="J209" t="s">
         <v>68</v>
@@ -14247,7 +14331,7 @@
         <v>1037</v>
       </c>
       <c r="H210" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="I210">
         <v>1665</v>
@@ -14300,7 +14384,7 @@
         <v>1037</v>
       </c>
       <c r="H211" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="J211" t="s">
         <v>76</v>
@@ -14547,7 +14631,7 @@
         <v>769</v>
       </c>
       <c r="E216" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="F216" t="s">
         <v>1037</v>
@@ -14653,7 +14737,7 @@
         <v>1037</v>
       </c>
       <c r="H218" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="I218">
         <v>10221</v>
@@ -14803,7 +14887,7 @@
         <v>1327057</v>
       </c>
       <c r="H221" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="I221">
         <v>1608817</v>
@@ -15047,7 +15131,7 @@
         <v>1037</v>
       </c>
       <c r="H226" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="I226">
         <v>6852544</v>
@@ -15097,7 +15181,7 @@
         <v>1037</v>
       </c>
       <c r="H227" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="I227">
         <v>166877</v>
@@ -15147,7 +15231,7 @@
         <v>1037</v>
       </c>
       <c r="H228" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="I228">
         <v>129028</v>
@@ -15200,7 +15284,7 @@
         <v>1037</v>
       </c>
       <c r="H229" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="I229">
         <v>317453</v>
@@ -15253,7 +15337,7 @@
         <v>1037</v>
       </c>
       <c r="H230" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="I230">
         <v>87117</v>
@@ -15306,7 +15390,7 @@
         <v>1037</v>
       </c>
       <c r="H231" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="I231">
         <v>433472</v>
@@ -15359,7 +15443,7 @@
         <v>1037</v>
       </c>
       <c r="H232" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="I232">
         <v>184716</v>
@@ -15412,7 +15496,7 @@
         <v>1037</v>
       </c>
       <c r="H233" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="I233">
         <v>18563</v>
@@ -15509,7 +15593,7 @@
         <v>1037</v>
       </c>
       <c r="H235" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="I235">
         <v>440167</v>
@@ -15759,7 +15843,7 @@
         <v>1037</v>
       </c>
       <c r="H240" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="I240">
         <v>360298</v>
@@ -16091,6 +16175,9 @@
       <c r="F246" t="s">
         <v>1037</v>
       </c>
+      <c r="H246" t="s">
+        <v>1112</v>
+      </c>
       <c r="I246">
         <v>22986</v>
       </c>
@@ -16247,8 +16334,11 @@
       <c r="E249" t="s">
         <v>1037</v>
       </c>
-      <c r="F249" t="s">
-        <v>1037</v>
+      <c r="F249" s="2">
+        <v>34175</v>
+      </c>
+      <c r="H249" t="s">
+        <v>1111</v>
       </c>
       <c r="I249">
         <v>5108079</v>
@@ -17080,8 +17170,8 @@
       <c r="E265" t="s">
         <v>289</v>
       </c>
-      <c r="H265" t="s">
-        <v>1086</v>
+      <c r="F265" s="2">
+        <v>17766</v>
       </c>
       <c r="I265">
         <v>18299</v>
@@ -17124,6 +17214,12 @@
       <c r="C266" t="s">
         <v>295</v>
       </c>
+      <c r="E266" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F266" t="s">
+        <v>1037</v>
+      </c>
       <c r="I266">
         <v>7241</v>
       </c>
@@ -17165,6 +17261,12 @@
       <c r="C267" t="s">
         <v>300</v>
       </c>
+      <c r="E267" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F267" t="s">
+        <v>1037</v>
+      </c>
       <c r="I267">
         <v>687</v>
       </c>
@@ -17206,6 +17308,12 @@
       <c r="C268" t="s">
         <v>302</v>
       </c>
+      <c r="E268" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F268" t="s">
+        <v>1037</v>
+      </c>
       <c r="I268">
         <v>551396</v>
       </c>
@@ -17247,6 +17355,12 @@
       <c r="C269" t="s">
         <v>305</v>
       </c>
+      <c r="E269" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F269" t="s">
+        <v>1037</v>
+      </c>
       <c r="I269">
         <v>4821</v>
       </c>
@@ -17288,6 +17402,12 @@
       <c r="C270" t="s">
         <v>310</v>
       </c>
+      <c r="E270" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F270" t="s">
+        <v>1037</v>
+      </c>
       <c r="I270">
         <v>368490</v>
       </c>
@@ -17329,6 +17449,15 @@
       <c r="C271" t="s">
         <v>364</v>
       </c>
+      <c r="E271" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F271" s="2">
+        <v>64274</v>
+      </c>
+      <c r="H271" t="s">
+        <v>1113</v>
+      </c>
       <c r="I271">
         <v>63149</v>
       </c>
@@ -17370,6 +17499,12 @@
       <c r="C272" t="s">
         <v>366</v>
       </c>
+      <c r="E272" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F272" t="s">
+        <v>1037</v>
+      </c>
       <c r="I272">
         <v>10114</v>
       </c>
@@ -17411,6 +17546,12 @@
       <c r="C273" t="s">
         <v>470</v>
       </c>
+      <c r="E273" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F273" t="s">
+        <v>1037</v>
+      </c>
       <c r="I273">
         <v>2697</v>
       </c>
@@ -17452,6 +17593,12 @@
       <c r="C274" t="s">
         <v>753</v>
       </c>
+      <c r="E274" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F274" t="s">
+        <v>1037</v>
+      </c>
       <c r="I274">
         <v>302402</v>
       </c>
@@ -17496,6 +17643,15 @@
       <c r="C275" t="s">
         <v>757</v>
       </c>
+      <c r="E275" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F275" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H275" t="s">
+        <v>1114</v>
+      </c>
       <c r="I275">
         <v>113309</v>
       </c>
@@ -17537,6 +17693,15 @@
       <c r="C276" t="s">
         <v>765</v>
       </c>
+      <c r="E276" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F276" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H276" t="s">
+        <v>1115</v>
+      </c>
       <c r="I276">
         <v>150912</v>
       </c>
@@ -17578,6 +17743,15 @@
       <c r="C277" t="s">
         <v>767</v>
       </c>
+      <c r="E277" t="s">
+        <v>746</v>
+      </c>
+      <c r="F277" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H277" t="s">
+        <v>1116</v>
+      </c>
       <c r="I277">
         <v>4341278</v>
       </c>
@@ -17619,6 +17793,12 @@
       <c r="C278" t="s">
         <v>774</v>
       </c>
+      <c r="E278" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F278" t="s">
+        <v>1037</v>
+      </c>
       <c r="I278">
         <v>2471</v>
       </c>
@@ -17660,6 +17840,12 @@
       <c r="C279" t="s">
         <v>793</v>
       </c>
+      <c r="E279" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F279" t="s">
+        <v>1037</v>
+      </c>
       <c r="I279">
         <v>15798</v>
       </c>
@@ -17701,6 +17887,12 @@
       <c r="C280" t="s">
         <v>796</v>
       </c>
+      <c r="E280" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F280" t="s">
+        <v>1037</v>
+      </c>
       <c r="I280">
         <v>688969</v>
       </c>
@@ -17745,6 +17937,12 @@
       <c r="C281" t="s">
         <v>799</v>
       </c>
+      <c r="E281" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F281" t="s">
+        <v>1037</v>
+      </c>
       <c r="I281">
         <v>31908</v>
       </c>
@@ -17786,6 +17984,12 @@
       <c r="C282" t="s">
         <v>802</v>
       </c>
+      <c r="E282" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F282" t="s">
+        <v>1037</v>
+      </c>
       <c r="I282">
         <v>3387429</v>
       </c>
@@ -17830,6 +18034,15 @@
       <c r="C283" t="s">
         <v>805</v>
       </c>
+      <c r="E283" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F283" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H283" t="s">
+        <v>1118</v>
+      </c>
       <c r="J283" t="s">
         <v>806</v>
       </c>
@@ -17868,6 +18081,12 @@
       <c r="C284" t="s">
         <v>807</v>
       </c>
+      <c r="E284" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F284" t="s">
+        <v>1037</v>
+      </c>
       <c r="I284">
         <v>150912</v>
       </c>
@@ -17909,6 +18128,12 @@
       <c r="C285" t="s">
         <v>810</v>
       </c>
+      <c r="E285" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F285" t="s">
+        <v>1037</v>
+      </c>
       <c r="I285">
         <v>398533</v>
       </c>
@@ -17953,6 +18178,12 @@
       <c r="C286" t="s">
         <v>813</v>
       </c>
+      <c r="E286" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F286" t="s">
+        <v>1037</v>
+      </c>
       <c r="I286">
         <v>2496953</v>
       </c>
@@ -17997,6 +18228,12 @@
       <c r="C287" t="s">
         <v>815</v>
       </c>
+      <c r="E287" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F287" t="s">
+        <v>1037</v>
+      </c>
       <c r="I287">
         <v>7664212</v>
       </c>
@@ -18041,6 +18278,12 @@
       <c r="C288" t="s">
         <v>870</v>
       </c>
+      <c r="E288" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F288" t="s">
+        <v>1037</v>
+      </c>
       <c r="I288">
         <v>22211549</v>
       </c>
@@ -18086,7 +18329,14 @@
         <v>1000</v>
       </c>
       <c r="E289" t="s">
-        <v>1000</v>
+        <v>1037</v>
+      </c>
+      <c r="F289">
+        <f>6483713+442543</f>
+        <v>6926256</v>
+      </c>
+      <c r="H289" t="s">
+        <v>1119</v>
       </c>
       <c r="I289">
         <v>12806975</v>
@@ -18129,6 +18379,15 @@
       <c r="C290" t="s">
         <v>99</v>
       </c>
+      <c r="E290" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F290">
+        <v>5295</v>
+      </c>
+      <c r="H290" t="s">
+        <v>1120</v>
+      </c>
       <c r="I290">
         <v>4717</v>
       </c>
@@ -18170,6 +18429,15 @@
       <c r="C291" t="s">
         <v>96</v>
       </c>
+      <c r="E291" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F291" s="2">
+        <v>11778</v>
+      </c>
+      <c r="H291" t="s">
+        <v>1121</v>
+      </c>
       <c r="I291">
         <v>29530</v>
       </c>
@@ -18211,6 +18479,15 @@
       <c r="C292" t="s">
         <v>186</v>
       </c>
+      <c r="E292" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F292" s="2">
+        <v>25096</v>
+      </c>
+      <c r="H292" t="s">
+        <v>1122</v>
+      </c>
       <c r="I292">
         <v>2839</v>
       </c>
@@ -18255,6 +18532,15 @@
       <c r="C293" t="s">
         <v>561</v>
       </c>
+      <c r="E293" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F293" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H293" t="s">
+        <v>1123</v>
+      </c>
       <c r="I293">
         <v>39122</v>
       </c>
@@ -18296,6 +18582,12 @@
       <c r="C294" t="s">
         <v>564</v>
       </c>
+      <c r="F294" s="2">
+        <v>91874</v>
+      </c>
+      <c r="H294" t="s">
+        <v>1124</v>
+      </c>
       <c r="I294">
         <v>61106</v>
       </c>
@@ -18337,6 +18629,12 @@
       <c r="C295" t="s">
         <v>675</v>
       </c>
+      <c r="E295" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F295" t="s">
+        <v>1037</v>
+      </c>
       <c r="I295">
         <v>5882</v>
       </c>
@@ -18381,6 +18679,15 @@
       <c r="C296" t="s">
         <v>830</v>
       </c>
+      <c r="E296" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F296" s="2">
+        <v>13134</v>
+      </c>
+      <c r="H296" t="s">
+        <v>1125</v>
+      </c>
       <c r="I296">
         <v>177</v>
       </c>
@@ -18425,6 +18732,15 @@
       <c r="C297" t="s">
         <v>107</v>
       </c>
+      <c r="E297" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F297" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H297" t="s">
+        <v>1127</v>
+      </c>
       <c r="I297">
         <v>10919</v>
       </c>
@@ -18531,6 +18847,12 @@
       <c r="C299" t="s">
         <v>157</v>
       </c>
+      <c r="E299" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F299" t="s">
+        <v>1037</v>
+      </c>
       <c r="I299">
         <v>70661</v>
       </c>
@@ -18576,7 +18898,14 @@
         <v>213</v>
       </c>
       <c r="E300" t="s">
-        <v>213</v>
+        <v>1037</v>
+      </c>
+      <c r="F300">
+        <f>435313+45655+7128</f>
+        <v>488096</v>
+      </c>
+      <c r="H300" t="s">
+        <v>1126</v>
       </c>
       <c r="I300">
         <v>46152</v>
@@ -18619,6 +18948,15 @@
       <c r="C301" t="s">
         <v>242</v>
       </c>
+      <c r="E301" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F301" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H301" t="s">
+        <v>1128</v>
+      </c>
       <c r="I301">
         <v>13935</v>
       </c>
@@ -18660,6 +18998,12 @@
       <c r="C302" t="s">
         <v>249</v>
       </c>
+      <c r="E302" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F302" t="s">
+        <v>1037</v>
+      </c>
       <c r="I302">
         <v>2390</v>
       </c>
@@ -18701,6 +19045,15 @@
       <c r="C303" t="s">
         <v>252</v>
       </c>
+      <c r="E303" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F303" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H303" t="s">
+        <v>1129</v>
+      </c>
       <c r="I303">
         <v>1429</v>
       </c>
@@ -18742,6 +19095,12 @@
       <c r="C304" t="s">
         <v>661</v>
       </c>
+      <c r="E304" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F304" t="s">
+        <v>1037</v>
+      </c>
       <c r="I304">
         <v>2114</v>
       </c>
@@ -18786,6 +19145,15 @@
       <c r="C305" t="s">
         <v>664</v>
       </c>
+      <c r="E305" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F305">
+        <v>6347010</v>
+      </c>
+      <c r="H305" t="s">
+        <v>1130</v>
+      </c>
       <c r="I305">
         <v>236</v>
       </c>
@@ -18830,6 +19198,15 @@
       <c r="C306" t="s">
         <v>667</v>
       </c>
+      <c r="E306" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F306" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H306" t="s">
+        <v>1131</v>
+      </c>
       <c r="J306" t="s">
         <v>668</v>
       </c>
@@ -18880,6 +19257,15 @@
       <c r="C307" t="s">
         <v>671</v>
       </c>
+      <c r="E307" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F307" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H307" t="s">
+        <v>1132</v>
+      </c>
       <c r="I307">
         <v>35848</v>
       </c>
@@ -18924,6 +19310,12 @@
       <c r="C308" t="s">
         <v>343</v>
       </c>
+      <c r="E308" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F308" t="s">
+        <v>1037</v>
+      </c>
       <c r="I308">
         <v>33456</v>
       </c>
@@ -18965,6 +19357,15 @@
       <c r="C309" t="s">
         <v>946</v>
       </c>
+      <c r="E309" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F309" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H309" t="s">
+        <v>1133</v>
+      </c>
       <c r="I309">
         <v>4000</v>
       </c>
@@ -19006,6 +19407,15 @@
       <c r="C310" t="s">
         <v>202</v>
       </c>
+      <c r="E310" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F310" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H310" t="s">
+        <v>1135</v>
+      </c>
       <c r="I310">
         <v>1331</v>
       </c>
@@ -19053,6 +19463,12 @@
       <c r="E311" t="s">
         <v>604</v>
       </c>
+      <c r="F311">
+        <v>935</v>
+      </c>
+      <c r="H311" t="s">
+        <v>604</v>
+      </c>
       <c r="I311">
         <v>3585</v>
       </c>
@@ -19094,6 +19510,12 @@
       <c r="C312" t="s">
         <v>206</v>
       </c>
+      <c r="E312" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F312" t="s">
+        <v>1037</v>
+      </c>
       <c r="I312">
         <v>10916</v>
       </c>
@@ -19135,6 +19557,12 @@
       <c r="C313" t="s">
         <v>368</v>
       </c>
+      <c r="E313" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F313" t="s">
+        <v>1037</v>
+      </c>
       <c r="I313">
         <v>218</v>
       </c>
@@ -19182,6 +19610,12 @@
       <c r="E314" t="s">
         <v>456</v>
       </c>
+      <c r="F314" s="2">
+        <v>23665</v>
+      </c>
+      <c r="H314" t="s">
+        <v>456</v>
+      </c>
       <c r="I314">
         <v>1898</v>
       </c>
@@ -19223,6 +19657,12 @@
       <c r="C315" t="s">
         <v>189</v>
       </c>
+      <c r="E315" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F315" t="s">
+        <v>1037</v>
+      </c>
       <c r="J315" t="s">
         <v>190</v>
       </c>
@@ -19261,6 +19701,12 @@
       <c r="C316" t="s">
         <v>236</v>
       </c>
+      <c r="E316" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F316" t="s">
+        <v>1037</v>
+      </c>
       <c r="I316">
         <v>248</v>
       </c>
@@ -19305,6 +19751,12 @@
       <c r="C317" t="s">
         <v>1013</v>
       </c>
+      <c r="E317" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F317" t="s">
+        <v>1037</v>
+      </c>
       <c r="I317">
         <v>25460</v>
       </c>
@@ -19352,6 +19804,12 @@
       <c r="E318" t="s">
         <v>59</v>
       </c>
+      <c r="F318" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H318" t="s">
+        <v>1136</v>
+      </c>
       <c r="I318">
         <v>339123</v>
       </c>
@@ -19397,7 +19855,13 @@
         <v>313</v>
       </c>
       <c r="E319" t="s">
-        <v>313</v>
+        <v>1137</v>
+      </c>
+      <c r="F319" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H319" t="s">
+        <v>1138</v>
       </c>
       <c r="I319">
         <v>5748</v>
@@ -19444,7 +19908,10 @@
         <v>313</v>
       </c>
       <c r="E320" t="s">
-        <v>313</v>
+        <v>1037</v>
+      </c>
+      <c r="F320" t="s">
+        <v>1037</v>
       </c>
       <c r="I320">
         <v>10062</v>
@@ -21903,6 +22370,9 @@
       </c>
       <c r="C377" t="s">
         <v>227</v>
+      </c>
+      <c r="H377" t="s">
+        <v>1110</v>
       </c>
       <c r="I377">
         <v>437515</v>

</xml_diff>

<commit_message>
Final transaction data matching
</commit_message>
<xml_diff>
--- a/data/processed/202308-services-list-processed - jbedits.xlsx
+++ b/data/processed/202308-services-list-processed - jbedits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Turing\Projects\decision-services-index\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDFCECB-6985-40FD-AD24-5000DE42995D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D281CAB8-E559-44F4-BD2D-694266C0C865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3757" uniqueCount="1153">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -3257,6 +3257,9 @@
     <t>UC combines Employment and Support Allowance, Jobseeker Allowance, Income Support, Child Tax Credit, Working Tax Credit and Housing Benefit. Only the first three are present in the data</t>
   </si>
   <si>
+    <t>Not present</t>
+  </si>
+  <si>
     <t>Not present in the web data. Child maintenance transactions are represented in the spreadsheet but not quite the same thing</t>
   </si>
   <si>
@@ -3437,12 +3440,6 @@
     <t>dataset access service</t>
   </si>
   <si>
-    <t>Should add together the three cells for applying for legal aid from the historical dataset</t>
-  </si>
-  <si>
-    <t>Legal aid in civil cases: acts of assistance, + 2 other similar rows to update</t>
-  </si>
-  <si>
     <t>Not the same as salmon rod catches which are used above</t>
   </si>
   <si>
@@ -3453,6 +3450,51 @@
   </si>
   <si>
     <t>This tribunal was rolled up into minor tribunal claims with a lot of other tribunal types. Make sure to only use this once here. No data on website</t>
+  </si>
+  <si>
+    <t>Bookings for prison visits</t>
+  </si>
+  <si>
+    <t>This is not legal aid which is about helping with defence</t>
+  </si>
+  <si>
+    <t>I think this is right - higher cases got to crown court. No data on website</t>
+  </si>
+  <si>
+    <t>I think this is right - I think this is for civil cases. No data on website</t>
+  </si>
+  <si>
+    <t>Present on the website but no data</t>
+  </si>
+  <si>
+    <t>Lasting Power of Attorney registrations</t>
+  </si>
+  <si>
+    <t>According to the detail on the website this is an aggregation of medex and matex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD MEDEX, MATEX etc. </t>
+  </si>
+  <si>
+    <t>Double checked and this is right. No data on website</t>
+  </si>
+  <si>
+    <t>Home childcarer registrations</t>
+  </si>
+  <si>
+    <t>Had a detailed look and I think this is nanny</t>
+  </si>
+  <si>
+    <t>This seems to be the same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think this register is new. Childcare registrations is below. </t>
+  </si>
+  <si>
+    <t>Provision of export credit guarantees and insurance policies</t>
+  </si>
+  <si>
+    <t>Applications for trade associations and other industry representative organisations to become accredited Trade Challenge Partners</t>
   </si>
 </sst>
 </file>
@@ -3839,10 +3881,10 @@
   <dimension ref="A1:W378"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B312" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B365" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A320" sqref="A320"/>
+      <selection pane="bottomRight" activeCell="H370" sqref="H370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3877,10 +3919,10 @@
         <v>1043</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -10075,7 +10117,7 @@
         <v>1037</v>
       </c>
       <c r="H124" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="I124">
         <v>1678413</v>
@@ -10128,7 +10170,7 @@
         <v>1037</v>
       </c>
       <c r="H125" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="I125">
         <v>83957</v>
@@ -10334,7 +10376,7 @@
         <v>1037</v>
       </c>
       <c r="H129" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="I129">
         <v>3432014</v>
@@ -10440,7 +10482,7 @@
         <v>37710</v>
       </c>
       <c r="H131" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="I131">
         <v>59478</v>
@@ -10493,7 +10535,7 @@
         <v>1037</v>
       </c>
       <c r="H132" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="I132">
         <v>49588</v>
@@ -10543,7 +10585,7 @@
         <v>282303</v>
       </c>
       <c r="H133" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="I133">
         <v>443305</v>
@@ -10596,7 +10638,7 @@
         <v>97000</v>
       </c>
       <c r="H134" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="I134">
         <v>282295</v>
@@ -10646,7 +10688,7 @@
         <v>1037</v>
       </c>
       <c r="H135" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="I135">
         <v>20724</v>
@@ -10746,7 +10788,7 @@
         <v>444119</v>
       </c>
       <c r="H137" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="I137">
         <v>43816</v>
@@ -10849,7 +10891,7 @@
         <v>182588</v>
       </c>
       <c r="H139" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="I139">
         <v>30377</v>
@@ -10899,7 +10941,7 @@
         <v>43760</v>
       </c>
       <c r="H140" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="I140">
         <v>15031</v>
@@ -10952,7 +10994,7 @@
         <v>1037</v>
       </c>
       <c r="H141" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="I141">
         <v>19493</v>
@@ -11293,7 +11335,7 @@
         <v>3921728</v>
       </c>
       <c r="H148" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="I148">
         <v>1012591</v>
@@ -13152,7 +13194,7 @@
         <v>535</v>
       </c>
       <c r="E186" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="F186" t="s">
         <v>1037</v>
@@ -13249,7 +13291,7 @@
         <v>554</v>
       </c>
       <c r="E188" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="F188" t="s">
         <v>1037</v>
@@ -13399,7 +13441,7 @@
         <v>1037</v>
       </c>
       <c r="H191" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="I191">
         <v>3270</v>
@@ -13458,7 +13500,7 @@
         <v>15118</v>
       </c>
       <c r="H192" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="I192">
         <v>10985</v>
@@ -13508,7 +13550,7 @@
         <v>1037</v>
       </c>
       <c r="H193" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="I193">
         <v>1946</v>
@@ -13608,7 +13650,7 @@
         <v>1037</v>
       </c>
       <c r="H195" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="I195">
         <v>231</v>
@@ -13705,7 +13747,7 @@
         <v>1037</v>
       </c>
       <c r="H197" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="I197">
         <v>193213</v>
@@ -13943,7 +13985,7 @@
         <v>1037</v>
       </c>
       <c r="H202" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="I202">
         <v>14577</v>
@@ -14081,7 +14123,7 @@
         <v>32787</v>
       </c>
       <c r="H205" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="I205">
         <v>39061</v>
@@ -14228,7 +14270,7 @@
         <v>58220</v>
       </c>
       <c r="H208" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="I208">
         <v>57316</v>
@@ -14275,13 +14317,13 @@
         <v>67</v>
       </c>
       <c r="E209" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="F209" t="s">
         <v>1037</v>
       </c>
       <c r="H209" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="J209" t="s">
         <v>68</v>
@@ -14331,7 +14373,7 @@
         <v>1037</v>
       </c>
       <c r="H210" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="I210">
         <v>1665</v>
@@ -14384,7 +14426,7 @@
         <v>1037</v>
       </c>
       <c r="H211" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="J211" t="s">
         <v>76</v>
@@ -14631,7 +14673,7 @@
         <v>769</v>
       </c>
       <c r="E216" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="F216" t="s">
         <v>1037</v>
@@ -14737,7 +14779,7 @@
         <v>1037</v>
       </c>
       <c r="H218" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="I218">
         <v>10221</v>
@@ -14887,7 +14929,7 @@
         <v>1327057</v>
       </c>
       <c r="H221" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="I221">
         <v>1608817</v>
@@ -15131,7 +15173,7 @@
         <v>1037</v>
       </c>
       <c r="H226" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="I226">
         <v>6852544</v>
@@ -15181,7 +15223,7 @@
         <v>1037</v>
       </c>
       <c r="H227" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="I227">
         <v>166877</v>
@@ -15231,7 +15273,7 @@
         <v>1037</v>
       </c>
       <c r="H228" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="I228">
         <v>129028</v>
@@ -15284,7 +15326,7 @@
         <v>1037</v>
       </c>
       <c r="H229" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="I229">
         <v>317453</v>
@@ -15337,7 +15379,7 @@
         <v>1037</v>
       </c>
       <c r="H230" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="I230">
         <v>87117</v>
@@ -15390,7 +15432,7 @@
         <v>1037</v>
       </c>
       <c r="H231" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="I231">
         <v>433472</v>
@@ -15443,7 +15485,7 @@
         <v>1037</v>
       </c>
       <c r="H232" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="I232">
         <v>184716</v>
@@ -15496,7 +15538,7 @@
         <v>1037</v>
       </c>
       <c r="H233" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="I233">
         <v>18563</v>
@@ -15593,7 +15635,7 @@
         <v>1037</v>
       </c>
       <c r="H235" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="I235">
         <v>440167</v>
@@ -15843,7 +15885,7 @@
         <v>1037</v>
       </c>
       <c r="H240" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="I240">
         <v>360298</v>
@@ -16176,7 +16218,7 @@
         <v>1037</v>
       </c>
       <c r="H246" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="I246">
         <v>22986</v>
@@ -16338,7 +16380,7 @@
         <v>34175</v>
       </c>
       <c r="H249" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="I249">
         <v>5108079</v>
@@ -17456,7 +17498,7 @@
         <v>64274</v>
       </c>
       <c r="H271" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="I271">
         <v>63149</v>
@@ -17650,7 +17692,7 @@
         <v>1037</v>
       </c>
       <c r="H275" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="I275">
         <v>113309</v>
@@ -17700,7 +17742,7 @@
         <v>1037</v>
       </c>
       <c r="H276" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="I276">
         <v>150912</v>
@@ -17750,7 +17792,7 @@
         <v>1037</v>
       </c>
       <c r="H277" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="I277">
         <v>4341278</v>
@@ -17794,7 +17836,7 @@
         <v>774</v>
       </c>
       <c r="E278" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="F278" t="s">
         <v>1037</v>
@@ -18041,7 +18083,7 @@
         <v>1037</v>
       </c>
       <c r="H283" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="J283" t="s">
         <v>806</v>
@@ -18336,7 +18378,7 @@
         <v>6926256</v>
       </c>
       <c r="H289" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="I289">
         <v>12806975</v>
@@ -18386,7 +18428,7 @@
         <v>5295</v>
       </c>
       <c r="H290" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="I290">
         <v>4717</v>
@@ -18436,7 +18478,7 @@
         <v>11778</v>
       </c>
       <c r="H291" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="I291">
         <v>29530</v>
@@ -18486,7 +18528,7 @@
         <v>25096</v>
       </c>
       <c r="H292" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="I292">
         <v>2839</v>
@@ -18539,7 +18581,7 @@
         <v>1037</v>
       </c>
       <c r="H293" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="I293">
         <v>39122</v>
@@ -18586,7 +18628,7 @@
         <v>91874</v>
       </c>
       <c r="H294" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="I294">
         <v>61106</v>
@@ -18686,7 +18728,7 @@
         <v>13134</v>
       </c>
       <c r="H296" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="I296">
         <v>177</v>
@@ -18739,7 +18781,7 @@
         <v>1037</v>
       </c>
       <c r="H297" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="I297">
         <v>10919</v>
@@ -18905,7 +18947,7 @@
         <v>488096</v>
       </c>
       <c r="H300" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="I300">
         <v>46152</v>
@@ -18955,7 +18997,7 @@
         <v>1037</v>
       </c>
       <c r="H301" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="I301">
         <v>13935</v>
@@ -19052,7 +19094,7 @@
         <v>1037</v>
       </c>
       <c r="H303" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="I303">
         <v>1429</v>
@@ -19152,7 +19194,7 @@
         <v>6347010</v>
       </c>
       <c r="H305" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="I305">
         <v>236</v>
@@ -19205,7 +19247,7 @@
         <v>1037</v>
       </c>
       <c r="H306" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="J306" t="s">
         <v>668</v>
@@ -19264,7 +19306,7 @@
         <v>1037</v>
       </c>
       <c r="H307" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="I307">
         <v>35848</v>
@@ -19358,13 +19400,13 @@
         <v>946</v>
       </c>
       <c r="E309" t="s">
-        <v>1134</v>
+        <v>348</v>
       </c>
       <c r="F309" t="s">
         <v>1037</v>
       </c>
       <c r="H309" t="s">
-        <v>1133</v>
+        <v>1141</v>
       </c>
       <c r="I309">
         <v>4000</v>
@@ -19414,7 +19456,7 @@
         <v>1037</v>
       </c>
       <c r="H310" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="I310">
         <v>1331</v>
@@ -19808,7 +19850,7 @@
         <v>1037</v>
       </c>
       <c r="H318" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="I318">
         <v>339123</v>
@@ -19855,13 +19897,13 @@
         <v>313</v>
       </c>
       <c r="E319" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F319" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H319" t="s">
         <v>1137</v>
-      </c>
-      <c r="F319" t="s">
-        <v>1037</v>
-      </c>
-      <c r="H319" t="s">
-        <v>1138</v>
       </c>
       <c r="I319">
         <v>5748</v>
@@ -19954,6 +19996,15 @@
       <c r="C321" t="s">
         <v>324</v>
       </c>
+      <c r="E321" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F321" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H321" t="s">
+        <v>1073</v>
+      </c>
       <c r="I321">
         <v>1126</v>
       </c>
@@ -20001,6 +20052,12 @@
       <c r="E322" t="s">
         <v>327</v>
       </c>
+      <c r="F322" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H322" t="s">
+        <v>1140</v>
+      </c>
       <c r="I322">
         <v>4249</v>
       </c>
@@ -20042,6 +20099,15 @@
       <c r="C323" t="s">
         <v>333</v>
       </c>
+      <c r="E323" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F323" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H323" t="s">
+        <v>1142</v>
+      </c>
       <c r="I323">
         <v>16241</v>
       </c>
@@ -20089,6 +20155,12 @@
       <c r="E324" t="s">
         <v>337</v>
       </c>
+      <c r="F324" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H324" t="s">
+        <v>1135</v>
+      </c>
       <c r="I324">
         <v>4084</v>
       </c>
@@ -20130,6 +20202,12 @@
       <c r="C325" t="s">
         <v>340</v>
       </c>
+      <c r="E325" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F325" t="s">
+        <v>1037</v>
+      </c>
       <c r="I325">
         <v>301136</v>
       </c>
@@ -20171,6 +20249,12 @@
       <c r="C326" t="s">
         <v>345</v>
       </c>
+      <c r="E326" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F326" t="s">
+        <v>1037</v>
+      </c>
       <c r="I326">
         <v>3123</v>
       </c>
@@ -20216,7 +20300,13 @@
         <v>348</v>
       </c>
       <c r="E327" t="s">
-        <v>348</v>
+        <v>1037</v>
+      </c>
+      <c r="F327" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H327" t="s">
+        <v>1139</v>
       </c>
       <c r="I327">
         <v>205056</v>
@@ -20259,6 +20349,12 @@
       <c r="C328" t="s">
         <v>350</v>
       </c>
+      <c r="E328" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F328" t="s">
+        <v>1037</v>
+      </c>
       <c r="I328">
         <v>32332</v>
       </c>
@@ -20300,6 +20396,12 @@
       <c r="C329" t="s">
         <v>355</v>
       </c>
+      <c r="E329" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F329" t="s">
+        <v>1037</v>
+      </c>
       <c r="I329">
         <v>147743</v>
       </c>
@@ -20341,6 +20443,12 @@
       <c r="C330" t="s">
         <v>370</v>
       </c>
+      <c r="E330" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F330" t="s">
+        <v>1037</v>
+      </c>
       <c r="I330">
         <v>3153</v>
       </c>
@@ -20382,6 +20490,15 @@
       <c r="C331" t="s">
         <v>951</v>
       </c>
+      <c r="E331" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F331" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H331" t="s">
+        <v>1119</v>
+      </c>
       <c r="I331">
         <v>264322</v>
       </c>
@@ -20423,6 +20540,12 @@
       <c r="C332" t="s">
         <v>953</v>
       </c>
+      <c r="F332" s="2">
+        <v>472797</v>
+      </c>
+      <c r="H332" t="s">
+        <v>1143</v>
+      </c>
       <c r="I332">
         <v>153514</v>
       </c>
@@ -20464,6 +20587,15 @@
       <c r="C333" t="s">
         <v>955</v>
       </c>
+      <c r="E333" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F333" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H333" t="s">
+        <v>1119</v>
+      </c>
       <c r="I333">
         <v>1245607</v>
       </c>
@@ -20508,6 +20640,15 @@
       <c r="C334" t="s">
         <v>958</v>
       </c>
+      <c r="E334" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F334">
+        <v>959421</v>
+      </c>
+      <c r="H334" t="s">
+        <v>1138</v>
+      </c>
       <c r="I334">
         <v>126038</v>
       </c>
@@ -20549,6 +20690,15 @@
       <c r="C335" t="s">
         <v>710</v>
       </c>
+      <c r="E335" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F335" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H335" t="s">
+        <v>1144</v>
+      </c>
       <c r="I335">
         <v>105936</v>
       </c>
@@ -20602,6 +20752,12 @@
       <c r="C336" t="s">
         <v>53</v>
       </c>
+      <c r="E336" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F336" t="s">
+        <v>1037</v>
+      </c>
       <c r="J336" t="s">
         <v>54</v>
       </c>
@@ -20640,6 +20796,12 @@
       <c r="C337" t="s">
         <v>860</v>
       </c>
+      <c r="E337" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F337" t="s">
+        <v>1037</v>
+      </c>
       <c r="J337" t="s">
         <v>861</v>
       </c>
@@ -20681,6 +20843,12 @@
       <c r="C338" t="s">
         <v>878</v>
       </c>
+      <c r="E338" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F338" t="s">
+        <v>1037</v>
+      </c>
       <c r="I338">
         <v>28197611</v>
       </c>
@@ -20725,6 +20893,12 @@
       <c r="C339" t="s">
         <v>895</v>
       </c>
+      <c r="E339" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F339" t="s">
+        <v>1037</v>
+      </c>
       <c r="I339">
         <v>101483774</v>
       </c>
@@ -20769,6 +20943,12 @@
       <c r="C340" t="s">
         <v>584</v>
       </c>
+      <c r="E340" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F340" t="s">
+        <v>1037</v>
+      </c>
       <c r="I340">
         <v>248</v>
       </c>
@@ -20810,6 +20990,12 @@
       <c r="C341" t="s">
         <v>199</v>
       </c>
+      <c r="E341" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F341" t="s">
+        <v>1037</v>
+      </c>
       <c r="I341">
         <v>301</v>
       </c>
@@ -20851,6 +21037,12 @@
       <c r="C342" t="s">
         <v>232</v>
       </c>
+      <c r="E342" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F342" t="s">
+        <v>1037</v>
+      </c>
       <c r="I342">
         <v>11515</v>
       </c>
@@ -20892,6 +21084,12 @@
       <c r="C343" t="s">
         <v>104</v>
       </c>
+      <c r="E343" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F343" t="s">
+        <v>1037</v>
+      </c>
       <c r="I343">
         <v>18692</v>
       </c>
@@ -20933,6 +21131,12 @@
       <c r="C344" t="s">
         <v>138</v>
       </c>
+      <c r="E344" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F344" t="s">
+        <v>1037</v>
+      </c>
       <c r="I344">
         <v>4533</v>
       </c>
@@ -20977,6 +21181,12 @@
       <c r="C345" t="s">
         <v>381</v>
       </c>
+      <c r="E345" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F345" t="s">
+        <v>1037</v>
+      </c>
       <c r="I345">
         <v>16165</v>
       </c>
@@ -21018,6 +21228,12 @@
       <c r="C346" t="s">
         <v>655</v>
       </c>
+      <c r="E346" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F346" t="s">
+        <v>1037</v>
+      </c>
       <c r="I346">
         <v>2222</v>
       </c>
@@ -21071,6 +21287,15 @@
       <c r="C347" t="s">
         <v>322</v>
       </c>
+      <c r="E347" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F347" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H347" t="s">
+        <v>1117</v>
+      </c>
       <c r="I347">
         <v>220282</v>
       </c>
@@ -21118,6 +21343,12 @@
       <c r="E348" t="s">
         <v>330</v>
       </c>
+      <c r="F348" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H348" t="s">
+        <v>1146</v>
+      </c>
       <c r="I348">
         <v>3347</v>
       </c>
@@ -21159,6 +21390,12 @@
       <c r="C349" t="s">
         <v>485</v>
       </c>
+      <c r="E349" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F349" t="s">
+        <v>1037</v>
+      </c>
       <c r="I349">
         <v>15800</v>
       </c>
@@ -21200,6 +21437,12 @@
       <c r="C350" t="s">
         <v>552</v>
       </c>
+      <c r="E350" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F350" t="s">
+        <v>1037</v>
+      </c>
       <c r="J350" t="s">
         <v>553</v>
       </c>
@@ -21242,7 +21485,13 @@
         <v>256</v>
       </c>
       <c r="E351" t="s">
-        <v>256</v>
+        <v>1037</v>
+      </c>
+      <c r="F351" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H351" t="s">
+        <v>1150</v>
       </c>
       <c r="I351">
         <v>3677</v>
@@ -21291,6 +21540,12 @@
       <c r="E352" t="s">
         <v>260</v>
       </c>
+      <c r="F352" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H352" t="s">
+        <v>1119</v>
+      </c>
       <c r="I352">
         <v>6716</v>
       </c>
@@ -21332,6 +21587,12 @@
       <c r="C353" t="s">
         <v>266</v>
       </c>
+      <c r="E353" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F353" t="s">
+        <v>1037</v>
+      </c>
       <c r="I353">
         <v>9938</v>
       </c>
@@ -21373,6 +21634,12 @@
       <c r="C354" t="s">
         <v>268</v>
       </c>
+      <c r="E354" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F354" t="s">
+        <v>1037</v>
+      </c>
       <c r="I354">
         <v>244793</v>
       </c>
@@ -21414,6 +21681,12 @@
       <c r="C355" t="s">
         <v>272</v>
       </c>
+      <c r="E355" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F355" t="s">
+        <v>1037</v>
+      </c>
       <c r="I355">
         <v>7059</v>
       </c>
@@ -21461,6 +21734,9 @@
       <c r="E356" t="s">
         <v>256</v>
       </c>
+      <c r="H356" t="s">
+        <v>1149</v>
+      </c>
       <c r="I356">
         <v>7376</v>
       </c>
@@ -21502,6 +21778,12 @@
       <c r="C357" t="s">
         <v>279</v>
       </c>
+      <c r="E357" t="s">
+        <v>1147</v>
+      </c>
+      <c r="H357" t="s">
+        <v>1148</v>
+      </c>
       <c r="I357">
         <v>3077</v>
       </c>
@@ -21543,6 +21825,12 @@
       <c r="C358" t="s">
         <v>281</v>
       </c>
+      <c r="E358" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F358" t="s">
+        <v>1037</v>
+      </c>
       <c r="I358">
         <v>61159</v>
       </c>
@@ -21584,6 +21872,15 @@
       <c r="C359" t="s">
         <v>548</v>
       </c>
+      <c r="E359" t="s">
+        <v>260</v>
+      </c>
+      <c r="F359" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H359" t="s">
+        <v>1117</v>
+      </c>
       <c r="I359">
         <v>8183</v>
       </c>
@@ -21625,6 +21922,9 @@
       <c r="C360" t="s">
         <v>864</v>
       </c>
+      <c r="E360" t="s">
+        <v>1037</v>
+      </c>
       <c r="I360">
         <v>2485</v>
       </c>
@@ -21669,6 +21969,12 @@
       <c r="C361" t="s">
         <v>529</v>
       </c>
+      <c r="E361" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F361" t="s">
+        <v>1037</v>
+      </c>
       <c r="I361">
         <v>25075</v>
       </c>
@@ -21710,6 +22016,12 @@
       <c r="C362" t="s">
         <v>849</v>
       </c>
+      <c r="E362" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F362" t="s">
+        <v>1037</v>
+      </c>
       <c r="I362">
         <v>540419</v>
       </c>
@@ -21852,6 +22164,12 @@
       <c r="C365" t="s">
         <v>539</v>
       </c>
+      <c r="E365" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F365" t="s">
+        <v>1037</v>
+      </c>
       <c r="I365">
         <v>687</v>
       </c>
@@ -21893,6 +22211,12 @@
       <c r="C366" t="s">
         <v>223</v>
       </c>
+      <c r="E366" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F366" t="s">
+        <v>1037</v>
+      </c>
       <c r="I366">
         <v>550011</v>
       </c>
@@ -21934,6 +22258,12 @@
       <c r="C367" t="s">
         <v>738</v>
       </c>
+      <c r="E367" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F367" t="s">
+        <v>1037</v>
+      </c>
       <c r="I367">
         <v>5417</v>
       </c>
@@ -21975,6 +22305,12 @@
       <c r="C368" t="s">
         <v>743</v>
       </c>
+      <c r="E368" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F368" t="s">
+        <v>1037</v>
+      </c>
       <c r="I368">
         <v>233418</v>
       </c>
@@ -22016,6 +22352,15 @@
       <c r="C369" t="s">
         <v>170</v>
       </c>
+      <c r="E369" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F369" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H369" t="s">
+        <v>1119</v>
+      </c>
       <c r="I369">
         <v>289</v>
       </c>
@@ -22060,6 +22405,12 @@
       <c r="C370" t="s">
         <v>246</v>
       </c>
+      <c r="F370">
+        <v>3</v>
+      </c>
+      <c r="H370" t="s">
+        <v>1152</v>
+      </c>
       <c r="J370" t="s">
         <v>247</v>
       </c>
@@ -22372,7 +22723,7 @@
         <v>227</v>
       </c>
       <c r="H377" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="I377">
         <v>437515</v>

</xml_diff>